<commit_message>
Styling options + full package creation without template
</commit_message>
<xml_diff>
--- a/CmdCore/Template.xlsx
+++ b/CmdCore/Template.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus\Desktop\stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
-    <sheet name="bla" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,41 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>d1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>d2</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,37 +37,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -104,47 +54,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -176,7 +94,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -188,7 +106,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -235,6 +153,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -270,6 +205,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,106 +374,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="F1">
-        <v>1.5</v>
-      </c>
-      <c r="G1" s="1">
-        <v>42736</v>
-      </c>
-      <c r="H1" s="2">
-        <v>42736.633483796293</v>
-      </c>
-      <c r="I1" s="5">
-        <v>43100</v>
-      </c>
-      <c r="J1" s="6">
-        <v>42736.633483796293</v>
-      </c>
-      <c r="K1">
-        <f>SUM(F1)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L1" s="3">
-        <v>5000</v>
-      </c>
-      <c r="M1" s="4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1.5</v>
-      </c>
-      <c r="G2" s="7">
-        <v>42736</v>
-      </c>
-      <c r="H2" s="8">
-        <v>42736.633483796293</v>
-      </c>
-      <c r="I2" s="9">
-        <v>43100</v>
-      </c>
-      <c r="J2" s="10">
-        <v>42736.633483796293</v>
-      </c>
-      <c r="K2" s="11">
-        <f>SUM(F2)</f>
-        <v>1.5</v>
-      </c>
-      <c r="L2" s="12">
-        <v>5000</v>
-      </c>
-      <c r="M2" s="13">
-        <v>0.05</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>